<commit_message>
3rd Commit For Fun
</commit_message>
<xml_diff>
--- a/ELEC 243 Lab/ELEC Lab Charts.xlsx
+++ b/ELEC 243 Lab/ELEC Lab Charts.xlsx
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -409,6 +409,41 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>